<commit_message>
Modelado Base de datos regla de juego
</commit_message>
<xml_diff>
--- a/doc/TORNEO.xlsx
+++ b/doc/TORNEO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="21195" windowHeight="9975"/>
@@ -265,8 +265,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +329,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,62 +523,71 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,7 +678,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -698,7 +712,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -874,14 +887,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
@@ -896,15 +909,15 @@
     <col min="14" max="14" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="32.25" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="5">
         <v>24</v>
       </c>
@@ -916,7 +929,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="5">
         <v>30</v>
       </c>
@@ -926,7 +939,7 @@
       <c r="C3" s="5"/>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" s="5">
         <v>32</v>
       </c>
@@ -936,7 +949,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" s="5">
         <v>36</v>
       </c>
@@ -946,7 +959,7 @@
       <c r="C5" s="5"/>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" s="5">
         <v>40</v>
       </c>
@@ -954,7 +967,7 @@
       <c r="C6" s="5"/>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" s="7">
         <v>45</v>
       </c>
@@ -964,7 +977,7 @@
       <c r="C7" s="7"/>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="5">
         <v>48</v>
       </c>
@@ -976,7 +989,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" s="7">
         <v>60</v>
       </c>
@@ -988,7 +1001,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="7">
         <v>72</v>
       </c>
@@ -1000,7 +1013,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="7">
         <v>96</v>
       </c>
@@ -1012,32 +1025,32 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+    <row r="14" spans="1:18">
+      <c r="A14" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="F14" s="39" t="s">
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="F14" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="41"/>
-      <c r="K14" s="39" t="s">
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
+      <c r="K14" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="41"/>
-      <c r="P14" s="42" t="s">
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="36"/>
+      <c r="P14" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="44"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q14" s="38"/>
+      <c r="R14" s="39"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="B15"/>
       <c r="P15" s="7" t="s">
         <v>75</v>
@@ -1049,12 +1062,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16" s="11"/>
       <c r="B16" s="16"/>
       <c r="C16" s="11"/>
       <c r="D16" s="7"/>
-      <c r="F16" s="34">
+      <c r="F16" s="33">
         <v>16</v>
       </c>
       <c r="G16" s="16" t="s">
@@ -1066,7 +1079,7 @@
       <c r="I16" s="7">
         <v>8</v>
       </c>
-      <c r="K16" s="34">
+      <c r="K16" s="33">
         <v>8</v>
       </c>
       <c r="L16" s="16" t="s">
@@ -1088,19 +1101,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F17" s="34"/>
-      <c r="G17" s="36" t="s">
+    <row r="17" spans="1:18">
+      <c r="F17" s="33"/>
+      <c r="G17" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="36" t="s">
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
       <c r="P17" s="7">
         <v>2</v>
       </c>
@@ -1111,7 +1124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" s="5">
         <v>30</v>
       </c>
@@ -1134,7 +1147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="P19" s="7">
         <v>4</v>
       </c>
@@ -1145,7 +1158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" s="30">
         <v>32</v>
       </c>
@@ -1158,7 +1171,7 @@
       <c r="D20" s="5">
         <v>16</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="33">
         <v>24</v>
       </c>
       <c r="G20" s="12" t="s">
@@ -1180,8 +1193,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F21" s="34"/>
+    <row r="21" spans="1:18">
+      <c r="F21" s="33"/>
       <c r="G21" s="12" t="s">
         <v>72</v>
       </c>
@@ -1201,7 +1214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="5">
         <v>36</v>
       </c>
@@ -1224,7 +1237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="P23" s="7">
         <v>8</v>
       </c>
@@ -1235,7 +1248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="5">
         <v>40</v>
       </c>
@@ -1248,7 +1261,7 @@
       <c r="D24" s="11">
         <v>24</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="41">
         <v>32</v>
       </c>
       <c r="G24" s="27" t="s">
@@ -1261,25 +1274,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="36" t="s">
+      <c r="F25" s="42"/>
+      <c r="G25" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="P25" s="42" t="s">
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="P25" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="44"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="37">
+      <c r="Q25" s="38"/>
+      <c r="R25" s="39"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="41">
         <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1301,8 +1314,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
+    <row r="27" spans="1:18">
+      <c r="A27" s="42"/>
       <c r="B27" s="3" t="s">
         <v>56</v>
       </c>
@@ -1322,7 +1335,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="9"/>
@@ -1337,8 +1350,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="34">
+    <row r="29" spans="1:18">
+      <c r="A29" s="33">
         <v>48</v>
       </c>
       <c r="B29" s="31" t="s">
@@ -1360,8 +1373,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+    <row r="30" spans="1:18">
+      <c r="A30" s="33"/>
       <c r="B30" s="31" t="s">
         <v>80</v>
       </c>
@@ -1381,8 +1394,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+    <row r="31" spans="1:18">
+      <c r="A31" s="33"/>
       <c r="B31" s="31" t="s">
         <v>79</v>
       </c>
@@ -1402,7 +1415,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18">
       <c r="P32" s="7">
         <v>6</v>
       </c>
@@ -1413,8 +1426,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="37">
+    <row r="33" spans="1:18">
+      <c r="A33" s="41">
         <v>64</v>
       </c>
       <c r="B33" s="16" t="s">
@@ -1436,8 +1449,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
+    <row r="34" spans="1:18">
+      <c r="A34" s="42"/>
       <c r="B34" s="31" t="s">
         <v>69</v>
       </c>
@@ -1457,7 +1470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18">
       <c r="P35" s="7">
         <v>9</v>
       </c>
@@ -1468,11 +1481,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="34">
+    <row r="36" spans="1:18">
+      <c r="A36" s="33">
         <v>72</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -1491,9 +1504,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
+    <row r="37" spans="1:18">
+      <c r="A37" s="33"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="11" t="s">
         <v>4</v>
       </c>
@@ -1510,7 +1523,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18">
       <c r="P38" s="7">
         <v>12</v>
       </c>
@@ -1521,11 +1534,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="34">
+    <row r="39" spans="1:18">
+      <c r="A39" s="33">
         <v>96</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -1544,9 +1557,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="35"/>
+    <row r="40" spans="1:18">
+      <c r="A40" s="33"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="11" t="s">
         <v>4</v>
       </c>
@@ -1563,8 +1576,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:18">
+      <c r="A41" s="33"/>
       <c r="B41" s="16" t="s">
         <v>74</v>
       </c>
@@ -1584,7 +1597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18">
       <c r="P42" s="7">
         <v>16</v>
       </c>
@@ -1597,6 +1610,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="P25:R25"/>
@@ -1611,12 +1630,6 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="G25:I25"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1624,19 +1637,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1">
       <c r="A1" s="19"/>
       <c r="B1" s="8" t="s">
         <v>25</v>
@@ -1675,7 +1688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1692,7 +1705,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1709,7 +1722,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1726,7 +1739,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1743,7 +1756,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1760,7 +1773,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1777,7 +1790,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1794,7 +1807,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1811,7 +1824,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1828,7 +1841,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1845,7 +1858,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1862,7 +1875,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1879,7 +1892,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1896,7 +1909,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1913,7 +1926,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1930,7 +1943,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1947,7 +1960,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1964,7 +1977,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1981,7 +1994,7 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1998,7 +2011,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -2015,7 +2028,7 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -2032,7 +2045,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -2049,7 +2062,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -2066,7 +2079,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2083,7 +2096,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -2100,7 +2113,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -2117,7 +2130,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -2134,7 +2147,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -2151,7 +2164,7 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -2168,7 +2181,7 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2185,7 +2198,7 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -2202,7 +2215,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" s="8">
         <v>32</v>
       </c>
@@ -2219,7 +2232,7 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="8">
         <v>33</v>
       </c>
@@ -2236,7 +2249,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" s="8">
         <v>34</v>
       </c>
@@ -2253,7 +2266,7 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="8">
         <v>35</v>
       </c>
@@ -2270,7 +2283,7 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="8">
         <v>36</v>
       </c>
@@ -2287,7 +2300,7 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="8">
         <v>37</v>
       </c>
@@ -2304,7 +2317,7 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" s="8">
         <v>38</v>
       </c>
@@ -2321,7 +2334,7 @@
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" s="8">
         <v>39</v>
       </c>
@@ -2338,7 +2351,7 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" s="8">
         <v>40</v>
       </c>
@@ -2355,7 +2368,7 @@
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" s="8">
         <v>41</v>
       </c>
@@ -2372,7 +2385,7 @@
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -2389,7 +2402,7 @@
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" s="8">
         <v>43</v>
       </c>
@@ -2406,7 +2419,7 @@
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" s="8">
         <v>44</v>
       </c>
@@ -2423,7 +2436,7 @@
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="8">
         <v>45</v>
       </c>
@@ -2440,7 +2453,7 @@
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" s="8">
         <v>46</v>
       </c>
@@ -2457,7 +2470,7 @@
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" s="8">
         <v>47</v>
       </c>
@@ -2474,7 +2487,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="8">
         <v>48</v>
       </c>
@@ -2491,7 +2504,7 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -2508,7 +2521,7 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="8">
         <v>50</v>
       </c>
@@ -2525,7 +2538,7 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" s="8">
         <v>51</v>
       </c>
@@ -2542,7 +2555,7 @@
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" s="8">
         <v>52</v>
       </c>
@@ -2559,7 +2572,7 @@
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="8">
         <v>53</v>
       </c>
@@ -2576,7 +2589,7 @@
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" s="8">
         <v>54</v>
       </c>
@@ -2593,7 +2606,7 @@
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="8">
         <v>55</v>
       </c>
@@ -2610,7 +2623,7 @@
       <c r="L56" s="6"/>
       <c r="M56" s="6"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="8">
         <v>56</v>
       </c>
@@ -2627,7 +2640,7 @@
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="8">
         <v>57</v>
       </c>
@@ -2644,7 +2657,7 @@
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="8">
         <v>58</v>
       </c>
@@ -2661,7 +2674,7 @@
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" s="8">
         <v>59</v>
       </c>
@@ -2678,7 +2691,7 @@
       <c r="L60" s="6"/>
       <c r="M60" s="6"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="8">
         <v>60</v>
       </c>
@@ -2701,21 +2714,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:P27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
@@ -2726,17 +2739,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="B3" s="18"/>
       <c r="C3" s="9"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="B4" s="18"/>
       <c r="C4" s="9"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="6" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="13" customFormat="1">
       <c r="A6" s="24" t="s">
         <v>27</v>
       </c>
@@ -2770,7 +2783,7 @@
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -2788,7 +2801,7 @@
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
@@ -2806,7 +2819,7 @@
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="15" t="s">
         <v>30</v>
       </c>
@@ -2824,7 +2837,7 @@
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2834,7 +2847,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -2844,37 +2857,37 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="13" customFormat="1">
       <c r="A12" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36" t="s">
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36" t="s">
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36" t="s">
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36" t="s">
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="8" t="s">
         <v>47</v>
       </c>
@@ -2924,7 +2937,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="23" t="s">
         <v>28</v>
       </c>
@@ -2964,7 +2977,7 @@
       </c>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="23" t="s">
         <v>29</v>
       </c>
@@ -3004,45 +3017,45 @@
       </c>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="G16" s="21"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="G17" s="21"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36" t="s">
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36" t="s">
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36" t="s">
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36" t="s">
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="8" t="s">
         <v>47</v>
       </c>
@@ -3092,7 +3105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="23" t="s">
         <v>28</v>
       </c>
@@ -3132,7 +3145,7 @@
       </c>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="23" t="s">
         <v>30</v>
       </c>
@@ -3172,7 +3185,7 @@
       </c>
       <c r="P21" s="6"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" s="25"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -3186,37 +3199,37 @@
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36" t="s">
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36" t="s">
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36" t="s">
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36" t="s">
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="8" t="s">
         <v>47</v>
       </c>
@@ -3266,7 +3279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" s="23" t="s">
         <v>29</v>
       </c>
@@ -3306,7 +3319,7 @@
       </c>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" s="23" t="s">
         <v>30</v>
       </c>
@@ -3348,6 +3361,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:J24"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:P12"/>
@@ -3358,11 +3376,6 @@
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3370,37 +3383,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="24" t="s">
         <v>62</v>
       </c>
@@ -3411,7 +3424,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="15">
         <v>1</v>
       </c>
@@ -3425,7 +3438,7 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="15">
         <v>2</v>
       </c>
@@ -3439,7 +3452,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="15">
         <v>3</v>
       </c>
@@ -3453,7 +3466,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="15">
         <v>4</v>
       </c>
@@ -3467,7 +3480,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="15">
         <v>5</v>
       </c>
@@ -3481,7 +3494,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="15">
         <v>6</v>
       </c>
@@ -3495,7 +3508,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="28"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -3503,7 +3516,7 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="28"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -3511,10 +3524,10 @@
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="13" t="s">
         <v>65</v>
       </c>
@@ -3525,22 +3538,22 @@
       <c r="C13" s="9"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="B14" s="18"/>
       <c r="C14" s="9"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="50" t="s">
+    <row r="15" spans="1:14">
+      <c r="C15" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="50" t="s">
+      <c r="D15" s="46"/>
+      <c r="E15" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="51"/>
-    </row>
-    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="46"/>
+    </row>
+    <row r="16" spans="1:14" s="13" customFormat="1">
       <c r="A16" s="24" t="s">
         <v>27</v>
       </c>
@@ -3578,7 +3591,7 @@
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="15" t="s">
         <v>28</v>
       </c>
@@ -3596,7 +3609,7 @@
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="15" t="s">
         <v>29</v>
       </c>
@@ -3614,7 +3627,7 @@
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="15" t="s">
         <v>30</v>
       </c>
@@ -3632,7 +3645,7 @@
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="15" t="s">
         <v>50</v>
       </c>
@@ -3650,7 +3663,7 @@
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
@@ -3660,7 +3673,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -3670,37 +3683,37 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="13" customFormat="1">
       <c r="A23" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49" t="s">
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49" t="s">
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49" t="s">
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="8" t="s">
         <v>47</v>
       </c>
@@ -3750,7 +3763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" s="23" t="str">
         <f>A17</f>
         <v>A</v>
@@ -3791,7 +3804,7 @@
       </c>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" s="23" t="s">
         <v>29</v>
       </c>
@@ -3831,45 +3844,45 @@
       </c>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="G27" s="21"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16">
       <c r="G28" s="21"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16">
       <c r="A29" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48" t="s">
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48" t="s">
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48" t="s">
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48" t="s">
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="8" t="s">
         <v>47</v>
       </c>
@@ -3919,7 +3932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" s="23" t="str">
         <f>A17</f>
         <v>A</v>
@@ -3960,7 +3973,7 @@
       </c>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16">
       <c r="A32" s="23" t="str">
         <f>A19</f>
         <v>C</v>
@@ -4001,37 +4014,37 @@
       </c>
       <c r="P32" s="6"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46" t="s">
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46" t="s">
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46" t="s">
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="L35" s="46"/>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46" t="s">
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="O35" s="46"/>
-      <c r="P35" s="46"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="8" t="s">
         <v>47</v>
       </c>
@@ -4081,7 +4094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" s="23" t="str">
         <f>A17</f>
         <v>A</v>
@@ -4122,7 +4135,7 @@
       </c>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="23" t="str">
         <f>A20</f>
         <v>D</v>
@@ -4163,7 +4176,7 @@
       </c>
       <c r="P38" s="6"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" s="25"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -4177,37 +4190,37 @@
       <c r="K40" s="25"/>
       <c r="L40" s="25"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47" t="s">
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47" t="s">
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47" t="s">
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47" t="s">
+      <c r="L41" s="50"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="O41" s="47"/>
-      <c r="P41" s="47"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O41" s="50"/>
+      <c r="P41" s="50"/>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="8" t="s">
         <v>47</v>
       </c>
@@ -4257,7 +4270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" s="23" t="str">
         <f>A18</f>
         <v>B</v>
@@ -4298,7 +4311,7 @@
       </c>
       <c r="P43" s="6"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="A44" s="23" t="str">
         <f>A19</f>
         <v>C</v>
@@ -4339,37 +4352,37 @@
       </c>
       <c r="P44" s="6"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="A47" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="45" t="s">
+      <c r="B47" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45" t="s">
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45" t="s">
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45" t="s">
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45" t="s">
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="O47" s="45"/>
-      <c r="P47" s="45"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="8" t="s">
         <v>47</v>
       </c>
@@ -4419,7 +4432,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="A49" s="23" t="str">
         <f>A18</f>
         <v>B</v>
@@ -4460,7 +4473,7 @@
       </c>
       <c r="P49" s="6"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="A50" s="23" t="str">
         <f>A20</f>
         <v>D</v>
@@ -4501,37 +4514,37 @@
       </c>
       <c r="P50" s="6"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="A53" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="46" t="s">
+      <c r="B53" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46" t="s">
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="46"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46" t="s">
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="I53" s="46"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="46" t="s">
+      <c r="I53" s="49"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="L53" s="46"/>
-      <c r="M53" s="46"/>
-      <c r="N53" s="46" t="s">
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="O53" s="46"/>
-      <c r="P53" s="46"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O53" s="49"/>
+      <c r="P53" s="49"/>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="8" t="s">
         <v>47</v>
       </c>
@@ -4581,7 +4594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="A55" s="23" t="str">
         <f>A19</f>
         <v>C</v>
@@ -4622,7 +4635,7 @@
       </c>
       <c r="P55" s="6"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="A56" s="23" t="str">
         <f>A20</f>
         <v>D</v>
@@ -4665,11 +4678,26 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:P35"/>
     <mergeCell ref="H29:J29"/>
     <mergeCell ref="K29:M29"/>
     <mergeCell ref="N29:P29"/>
@@ -4678,26 +4706,11 @@
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="N23:P23"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Modelado de db en DJANGO models.py
</commit_message>
<xml_diff>
--- a/doc/TORNEO.xlsx
+++ b/doc/TORNEO.xlsx
@@ -12,12 +12,12 @@
     <sheet name="GRUPOS 3" sheetId="3" r:id="rId3"/>
     <sheet name="GRUPOS 4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="84">
   <si>
     <t>PRIMERA FASE</t>
   </si>
@@ -260,13 +260,22 @@
   </si>
   <si>
     <t>12 GRUPOS DE 4</t>
+  </si>
+  <si>
+    <t>10*2=20</t>
+  </si>
+  <si>
+    <t>4 DEFINE A PUNTAJE?</t>
+  </si>
+  <si>
+    <t>clasif 2 x grupo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +287,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -429,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,9 +539,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -544,20 +575,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,28 +605,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -890,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -913,8 +936,8 @@
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="E1"/>
     </row>
     <row r="2" spans="1:18">
@@ -1026,29 +1049,29 @@
       <c r="E11"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
-      <c r="F14" s="52" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="F14" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
-      <c r="K14" s="34" t="s">
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="47"/>
+      <c r="K14" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="36"/>
-      <c r="P14" s="37" t="s">
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
+      <c r="P14" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="39"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="44"/>
     </row>
     <row r="15" spans="1:18">
       <c r="B15"/>
@@ -1064,10 +1087,12 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="11"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="57" t="s">
+        <v>83</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="7"/>
-      <c r="F16" s="33">
+      <c r="F16" s="34">
         <v>16</v>
       </c>
       <c r="G16" s="16" t="s">
@@ -1079,7 +1104,7 @@
       <c r="I16" s="7">
         <v>8</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K16" s="34">
         <v>8</v>
       </c>
       <c r="L16" s="16" t="s">
@@ -1102,18 +1127,24 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="F17" s="33"/>
-      <c r="G17" s="40" t="s">
+      <c r="B17" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="34"/>
+      <c r="G17" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="40" t="s">
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
       <c r="P17" s="7">
         <v>2</v>
       </c>
@@ -1171,7 +1202,7 @@
       <c r="D20" s="5">
         <v>16</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="34">
         <v>24</v>
       </c>
       <c r="G20" s="12" t="s">
@@ -1194,7 +1225,7 @@
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="F21" s="33"/>
+      <c r="F21" s="34"/>
       <c r="G21" s="12" t="s">
         <v>72</v>
       </c>
@@ -1261,7 +1292,7 @@
       <c r="D24" s="11">
         <v>24</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="37">
         <v>32</v>
       </c>
       <c r="G24" s="27" t="s">
@@ -1279,20 +1310,20 @@
       <c r="B25" s="18"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="40" t="s">
+      <c r="F25" s="38"/>
+      <c r="G25" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="P25" s="37" t="s">
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="P25" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="39"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="44"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="41">
+      <c r="A26" s="37">
         <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1315,7 +1346,7 @@
       </c>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="42"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="3" t="s">
         <v>56</v>
       </c>
@@ -1351,7 +1382,7 @@
       </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="33">
+      <c r="A29" s="34">
         <v>48</v>
       </c>
       <c r="B29" s="31" t="s">
@@ -1374,7 +1405,7 @@
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="33"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="31" t="s">
         <v>80</v>
       </c>
@@ -1395,7 +1426,7 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="33"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="31" t="s">
         <v>79</v>
       </c>
@@ -1427,7 +1458,7 @@
       </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="41">
+      <c r="A33" s="37">
         <v>64</v>
       </c>
       <c r="B33" s="16" t="s">
@@ -1450,7 +1481,7 @@
       </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="42"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="31" t="s">
         <v>69</v>
       </c>
@@ -1482,10 +1513,10 @@
       </c>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="33">
+      <c r="A36" s="34">
         <v>72</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="35" t="s">
         <v>66</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -1505,8 +1536,8 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="33"/>
-      <c r="B37" s="43"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="11" t="s">
         <v>4</v>
       </c>
@@ -1535,10 +1566,10 @@
       </c>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="33">
+      <c r="A39" s="34">
         <v>96</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="35" t="s">
         <v>68</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -1558,8 +1589,8 @@
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="33"/>
-      <c r="B40" s="43"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="11" t="s">
         <v>4</v>
       </c>
@@ -1577,7 +1608,7 @@
       </c>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="33"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="16" t="s">
         <v>74</v>
       </c>
@@ -1610,12 +1641,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="P25:R25"/>
@@ -1630,9 +1655,15 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2861,31 +2892,31 @@
       <c r="A12" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40" t="s">
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40" t="s">
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40" t="s">
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="8" t="s">
@@ -3029,31 +3060,31 @@
       <c r="A18" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40" t="s">
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40" t="s">
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40" t="s">
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="8" t="s">
@@ -3203,31 +3234,31 @@
       <c r="A24" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40" t="s">
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40" t="s">
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40" t="s">
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40" t="s">
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="8" t="s">
@@ -3361,11 +3392,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:J24"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:P12"/>
@@ -3376,6 +3402,11 @@
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:G12"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3410,10 +3441,10 @@
       <c r="A3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="24" t="s">
         <v>62</v>
       </c>
@@ -3544,14 +3575,14 @@
       <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="45" t="s">
+      <c r="D15" s="54"/>
+      <c r="E15" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="46"/>
+      <c r="F15" s="54"/>
     </row>
     <row r="16" spans="1:14" s="13" customFormat="1">
       <c r="A16" s="24" t="s">
@@ -3687,31 +3718,31 @@
       <c r="A23" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48" t="s">
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48" t="s">
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48" t="s">
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48" t="s">
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="52"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="8" t="s">
@@ -3856,31 +3887,31 @@
       <c r="A29" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47" t="s">
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47" t="s">
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47" t="s">
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47" t="s">
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="8" t="s">
@@ -4356,31 +4387,31 @@
       <c r="A47" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51" t="s">
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="51" t="s">
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51" t="s">
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="L47" s="51"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="51" t="s">
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="O47" s="51"/>
-      <c r="P47" s="51"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="8" t="s">
@@ -4678,26 +4709,11 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
     <mergeCell ref="H29:J29"/>
     <mergeCell ref="K29:M29"/>
     <mergeCell ref="N29:P29"/>
@@ -4706,11 +4722,26 @@
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="N23:P23"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="N47:P47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>